<commit_message>
regex with unicode accents
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -32,7 +32,7 @@
   </si>
   <si>
     <t xml:space="preserve"> @FFAAECUADOR: #Quito| La Primera Division de Ejercito Shyris, realizo 
-120 pruebas rapidas y 38 pruebas PCR de #Covid_19, a los militares,""</t>
+120 pruebas rapidas y 38 pruebas PCR de #Covid_19, a los militares,"" hóla múndo 😂 ⛔️ ñ</t>
   </si>
   <si>
     <t xml:space="preserve">positivo</t>
@@ -6459,11 +6459,11 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A218" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A221" activeCellId="0" sqref="A221"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="158.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21"/>
@@ -10763,7 +10763,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="538" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="538" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A538" s="2" t="s">
         <v>403</v>
       </c>

</xml_diff>